<commit_message>
quick job time report
</commit_message>
<xml_diff>
--- a/orion.web/docs/QuickJobTimeReport.xlsx
+++ b/orion.web/docs/QuickJobTimeReport.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\orion-web\orion.web\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF91BEC2-965D-4556-BF10-B25C2B376CC3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2C3AE4-6297-4B71-B937-093E66592864}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{CE18695A-0F8A-43C1-A856-081F54D40452}"/>
   </bookViews>
   <sheets>
-    <sheet name="ProjectStatusReport" sheetId="1" r:id="rId1"/>
+    <sheet name="QuickJobTimeReport" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,12 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>GM M5 Project  (Silao)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BARTON MALOW </t>
-  </si>
-  <si>
     <t>XXXX</t>
   </si>
   <si>
@@ -64,13 +58,19 @@
   </si>
   <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>Job Name</t>
+  </si>
+  <si>
+    <t>Client Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,8 +110,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,12 +128,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -192,8 +193,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -209,9 +211,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -221,21 +220,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -254,9 +247,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{F0C5D127-2787-4824-BAF1-559AF0AFDF55}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -571,7 +574,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,70 +589,72 @@
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="12"/>
+      <c r="C1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16"/>
+      <c r="D2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19"/>
+        <v>7</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>8</v>
+      <c r="A5" s="18"/>
+      <c r="B5" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="D3:F3"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
sub-total and grand-total on quick job report
</commit_message>
<xml_diff>
--- a/orion.web/docs/QuickJobTimeReport.xlsx
+++ b/orion.web/docs/QuickJobTimeReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\orion-web\orion.web\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2C3AE4-6297-4B71-B937-093E66592864}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398D8BF3-D754-4BC0-8DE4-A38C9F10BB81}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{CE18695A-0F8A-43C1-A856-081F54D40452}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{CE18695A-0F8A-43C1-A856-081F54D40452}"/>
   </bookViews>
   <sheets>
     <sheet name="QuickJobTimeReport" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>XXXX</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Client Name</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -217,8 +220,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -246,12 +255,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -571,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C40B4EC7-15E3-4156-9BB2-857B3430EBF4}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,23 +588,24 @@
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="10"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
     </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -611,42 +615,45 @@
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
     </row>
-    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="16"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
-      <c r="B5" s="17" t="s">
+    <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9"/>
+      <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="19"/>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="8" t="s">
         <v>6</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>